<commit_message>
update errors in parameter values
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4CE006-66A8-41F2-9A24-1E3376C64312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C4765-EBB2-46C6-BE46-A4FEFAE391C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="2880" yWindow="2895" windowWidth="16740" windowHeight="13620" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter values" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -243,13 +243,7 @@
     <t>Baniasadi, M. et al. Waste to energy valorization of poultry litter by slow pyrolysis. Renewable Energy 90, 458â468 (2016).</t>
   </si>
   <si>
-    <t>Atienza-MartÃ­nez, M., Ãbrego, J., Gea, G. &amp; MarÃ­as, F. Pyrolysis of dairy cattle manure: evolution of char characteristics. Journal of Analytical and Applied Pyrolysis 145, 104724 (2020).</t>
-  </si>
-  <si>
     <t>Uzoma, K.C., Inoue, M., Andry, H., Fujimaki, H., Zahoor, A. and Nishihara, E., 2011. Effect of cow manure biochar on maize productivity under sandy soil condition. Soil use and management, 27(2), pp.205-212.</t>
-  </si>
-  <si>
-    <t>low value is the lowest value reported in the paper, default is the highest value. Difference between the 2 reported values is added to the default value to calculate the high value</t>
   </si>
   <si>
     <t>Tsai, W.T., Liu, S.C., Chen, H.R., Chang, Y.M. and Tsai, Y.L., 2012. Textural and chemical properties of swine-manure-derived biochar pertinent to its potential use as a soil amendment. Chemosphere, 89(2), pp.198-203.</t>
@@ -516,9 +510,6 @@
     <t>Cayuela, M.L., Van Zwieten, L., Singh, B.P., Jeffery, S., Roig, A. and Sánchez-Monedero, M.A., 2014. Biochar's role in mitigating soil nitrous oxide emissions: A review and meta-analysis. Agriculture, Ecosystems &amp; Environment, 191, pp.5-16.</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -552,27 +543,9 @@
     <t>Adoption70</t>
   </si>
   <si>
-    <t>CarbonTaxA</t>
-  </si>
-  <si>
-    <t>CarbonTaxB</t>
-  </si>
-  <si>
-    <t>BiocharSubsidyA</t>
-  </si>
-  <si>
-    <t>BiocharSubsidyB</t>
-  </si>
-  <si>
     <t>save all log files</t>
   </si>
   <si>
-    <t>CarbonStabilityA</t>
-  </si>
-  <si>
-    <t>CarbonStabilityB</t>
-  </si>
-  <si>
     <t>World Bank Group. State and Trends of Carbon Pricing Dashboard. State and Trends of Carbon Pricing Dashboard. https://carbonpricingdashboard.worldbank.org/compliance/price (accessed 2025-10-29).</t>
   </si>
   <si>
@@ -586,6 +559,36 @@
   </si>
   <si>
     <t>config files made</t>
+  </si>
+  <si>
+    <t>CarbonTaxLow</t>
+  </si>
+  <si>
+    <t>CarbonTaxHigh</t>
+  </si>
+  <si>
+    <t>BiocharSubsidyLow</t>
+  </si>
+  <si>
+    <t>BiocharSubsidyHigh</t>
+  </si>
+  <si>
+    <t>CarbonStabilityLow</t>
+  </si>
+  <si>
+    <t>CarbonStabilityHigh</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>need to reset L142?</t>
+  </si>
+  <si>
+    <t>Zhou, S., Liang, H., Han, L., Huang, G. and Yang, Z., 2019. The influence of manure feedstock, slow pyrolysis, and hydrothermal temperature on manure thermochemical and combustion properties. Waste management, 88, pp.85-95.</t>
+  </si>
+  <si>
+    <t>default is median at 500C. Low is minimum yield at 600C, High is maximum yield at 400C.</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +652,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,36 +727,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,6 +764,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1094,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,30 +1155,29 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="D2" s="6">
-        <f>C2*2-B2</f>
-        <v>0.502</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="B2" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1179,16 +1197,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1207,43 +1225,41 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="D5" s="6">
-        <f>D2</f>
-        <v>0.502</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="4" t="str">
-        <f>G2</f>
-        <v>low value is the lowest value reported in the paper, default is the highest value. Difference between the 2 reported values is added to the default value to calculate the high value</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="B5" s="16">
+        <v>0.34470000000000001</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.43009999999999998</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.53129999999999999</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1264,16 +1280,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1293,16 +1309,16 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1319,10 +1335,10 @@
         <v>0.56110000000000004</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>6</v>
@@ -1347,16 +1363,16 @@
         <v>5.2500000000000003E-3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1375,41 +1391,41 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="16">
         <v>0.42949999999999999</v>
       </c>
-      <c r="C11" s="6">
-        <v>0.46820000000000001</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="16">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="D11" s="16">
         <v>0.54679999999999995</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1427,16 +1443,16 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1453,16 +1469,16 @@
         <v>3.1E-2</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1479,7 +1495,7 @@
         <v>0.53259999999999996</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>67</v>
@@ -1507,16 +1523,16 @@
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1535,16 +1551,16 @@
         <v>7.46E-2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1679,7 +1695,7 @@
     </row>
     <row r="22" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" s="7">
         <f>0.5*C22</f>
@@ -1696,10 +1712,10 @@
         <v>49</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>64</v>
@@ -1707,7 +1723,7 @@
     </row>
     <row r="23" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" s="7">
         <f t="shared" ref="B23:B36" si="0">0.5*C23</f>
@@ -1724,10 +1740,10 @@
         <v>49</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>64</v>
@@ -1735,7 +1751,7 @@
     </row>
     <row r="24" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" s="7">
         <f t="shared" si="0"/>
@@ -1752,10 +1768,10 @@
         <v>49</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>64</v>
@@ -1763,7 +1779,7 @@
     </row>
     <row r="25" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" s="7">
         <f t="shared" si="0"/>
@@ -1780,10 +1796,10 @@
         <v>49</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>64</v>
@@ -1791,7 +1807,7 @@
     </row>
     <row r="26" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" s="7">
         <f t="shared" si="0"/>
@@ -1808,10 +1824,10 @@
         <v>49</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>64</v>
@@ -1836,10 +1852,10 @@
         <v>60</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>64</v>
@@ -1864,10 +1880,10 @@
         <v>60</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>64</v>
@@ -1892,10 +1908,10 @@
         <v>60</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>64</v>
@@ -1920,10 +1936,10 @@
         <v>60</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>64</v>
@@ -1948,10 +1964,10 @@
         <v>60</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>64</v>
@@ -1976,10 +1992,10 @@
         <v>61</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>64</v>
@@ -2004,10 +2020,10 @@
         <v>61</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>64</v>
@@ -2032,10 +2048,10 @@
         <v>61</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>64</v>
@@ -2060,10 +2076,10 @@
         <v>61</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>64</v>
@@ -2088,10 +2104,10 @@
         <v>61</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>64</v>
@@ -2114,13 +2130,13 @@
         <v>31</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -2140,13 +2156,13 @@
         <v>31</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2166,18 +2182,18 @@
         <v>31</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" s="7">
         <v>1E-3</v>
@@ -2189,16 +2205,16 @@
         <v>0.1</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>65</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2218,18 +2234,18 @@
         <v>31</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B42" s="10">
         <v>250</v>
@@ -2241,21 +2257,21 @@
         <v>2500</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" s="11">
         <v>2.1999999999999999E-2</v>
@@ -2270,18 +2286,18 @@
         <v>31</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" s="11">
         <v>5.5E-2</v>
@@ -2296,18 +2312,18 @@
         <v>31</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B45" s="11">
         <v>5.5E-2</v>
@@ -2322,18 +2338,18 @@
         <v>31</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B46" s="11">
         <v>5.5E-2</v>
@@ -2348,18 +2364,18 @@
         <v>31</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" s="11">
         <v>5.5E-2</v>
@@ -2374,18 +2390,18 @@
         <v>31</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" s="11">
         <v>8.2000000000000003E-2</v>
@@ -2400,18 +2416,18 @@
         <v>31</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" s="11">
         <v>5.5E-2</v>
@@ -2426,18 +2442,18 @@
         <v>31</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" s="11">
         <v>5.5E-2</v>
@@ -2452,18 +2468,18 @@
         <v>31</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" s="11">
         <v>5.5E-2</v>
@@ -2478,18 +2494,18 @@
         <v>31</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" s="11">
         <v>-1.0999999999999999E-2</v>
@@ -2504,18 +2520,18 @@
         <v>31</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B53" s="11">
         <v>5.5E-2</v>
@@ -2530,18 +2546,18 @@
         <v>31</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B54" s="11">
         <v>1.6E-2</v>
@@ -2556,18 +2572,18 @@
         <v>31</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B55" s="11">
         <v>4.9000000000000002E-2</v>
@@ -2582,18 +2598,18 @@
         <v>31</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B56" s="11">
         <v>5.5E-2</v>
@@ -2608,18 +2624,18 @@
         <v>31</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B57" s="11">
         <v>5.5E-2</v>
@@ -2634,18 +2650,18 @@
         <v>31</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B58" s="11">
         <v>5.0000000000000001E-3</v>
@@ -2660,18 +2676,18 @@
         <v>31</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" s="11">
         <f>B52</f>
@@ -2689,18 +2705,18 @@
         <v>31</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B60" s="11">
         <v>5.5E-2</v>
@@ -2715,18 +2731,18 @@
         <v>31</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B61" s="11">
         <v>5.5E-2</v>
@@ -2741,18 +2757,18 @@
         <v>31</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B62" s="11">
         <v>5.5E-2</v>
@@ -2767,18 +2783,18 @@
         <v>31</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B63" s="13">
         <v>0.3</v>
@@ -2793,18 +2809,18 @@
         <v>31</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B64" s="1">
         <v>12.84</v>
@@ -2816,21 +2832,21 @@
         <v>136.03</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B65" s="1">
         <v>50</v>
@@ -2842,21 +2858,21 @@
         <v>150</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B66" s="13">
         <v>0.33</v>
@@ -2871,10 +2887,10 @@
         <v>31</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>64</v>
@@ -2890,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2902,7 +2918,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2910,218 +2926,221 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" t="s">
-        <v>160</v>
+        <v>165</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>139</v>
       </c>
-      <c r="B16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>140</v>
       </c>
-      <c r="B17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>142</v>
       </c>
-      <c r="B19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
yields updated in config files
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C4765-EBB2-46C6-BE46-A4FEFAE391C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFC40D9-86E5-4E05-95E6-6BFEBBEB5B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2895" windowWidth="16740" windowHeight="13620" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="6360" yWindow="1155" windowWidth="11835" windowHeight="13620" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter values" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -144,33 +144,12 @@
     <t xml:space="preserve">$1975/kg biochar </t>
   </si>
   <si>
-    <t>0.0196 @ 5% interest rate</t>
-  </si>
-  <si>
-    <t>0.0257 @ 12% interest rate</t>
-  </si>
-  <si>
-    <t>0.0339 @ 20% interest rate</t>
-  </si>
-  <si>
-    <t>0.0189 @ 5% interest rate</t>
-  </si>
-  <si>
-    <t>0.0248 @ 12% interest rate</t>
-  </si>
-  <si>
-    <t>0.0328 @ 20% interest rate</t>
-  </si>
-  <si>
     <t>0.0184 @ 5% interest rate</t>
   </si>
   <si>
     <t>0.0320 @ 20% interest rate</t>
   </si>
   <si>
-    <t>0.0192 @ 5% interest rate</t>
-  </si>
-  <si>
     <t>0.0252 @ 12% interest rate</t>
   </si>
   <si>
@@ -186,9 +165,6 @@
     <t>0.0331 @ 20% interest rate</t>
   </si>
   <si>
-    <t>kg C/kg biochar</t>
-  </si>
-  <si>
     <t>Beef Biochar Avoided CH4</t>
   </si>
   <si>
@@ -349,21 +325,6 @@
   </si>
   <si>
     <t>A_agBiocharCropYieldIncrease</t>
-  </si>
-  <si>
-    <t>Beef Biochar Net C</t>
-  </si>
-  <si>
-    <t>Dairy Biochar Net C</t>
-  </si>
-  <si>
-    <t>Goat Biochar Net C</t>
-  </si>
-  <si>
-    <t>Pork Biochar Net C</t>
-  </si>
-  <si>
-    <t>Poultry Biochar Net C</t>
   </si>
   <si>
     <t>kg biochar/ha</t>
@@ -589,6 +550,24 @@
   </si>
   <si>
     <t>default is median at 500C. Low is minimum yield at 600C, High is maximum yield at 400C.</t>
+  </si>
+  <si>
+    <t>0.0254 @ 12% interest rate</t>
+  </si>
+  <si>
+    <t>0.0274 @ 12% interest rate</t>
+  </si>
+  <si>
+    <t>0.0193 @ 5% interest rate</t>
+  </si>
+  <si>
+    <t>0.0209 @ 5% interest rate</t>
+  </si>
+  <si>
+    <t>0.0335 @ 20% interest rate</t>
+  </si>
+  <si>
+    <t>0.0362 @ 20% interest rate</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1169,16 +1148,16 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1197,16 +1176,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1225,16 +1204,16 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1251,16 +1230,16 @@
         <v>0.53129999999999999</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1280,16 +1259,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1309,16 +1288,16 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1335,16 +1314,16 @@
         <v>0.56110000000000004</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1363,16 +1342,16 @@
         <v>5.2500000000000003E-3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1391,16 +1370,16 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="14" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1417,16 +1396,16 @@
         <v>0.54679999999999995</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1443,16 +1422,16 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,16 +1448,16 @@
         <v>3.1E-2</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1495,16 +1474,16 @@
         <v>0.53259999999999996</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1523,16 +1502,16 @@
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1551,68 +1530,68 @@
         <v>7.46E-2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>156</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>157</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1620,684 +1599,674 @@
         <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="7">
-        <f>0.5*C22</f>
-        <v>-0.125</v>
-      </c>
-      <c r="C22" s="7">
-        <v>-0.25</v>
-      </c>
-      <c r="D22" s="7">
-        <f>1.5*C22</f>
-        <v>-0.375</v>
+        <v>42</v>
+      </c>
+      <c r="B22" s="8">
+        <f t="shared" ref="B22:B31" si="0">0.5*C22</f>
+        <v>-5.2500000000000003E-3</v>
+      </c>
+      <c r="C22" s="8">
+        <v>-1.0500000000000001E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <f t="shared" ref="D22:D31" si="1">1.5*C22</f>
+        <v>-1.575E-2</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="7">
-        <f t="shared" ref="B23:B36" si="0">0.5*C23</f>
-        <v>-0.125</v>
-      </c>
-      <c r="C23" s="7">
-        <v>-0.25</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" ref="D23:D36" si="1">1.5*C23</f>
-        <v>-0.375</v>
+        <v>43</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" si="0"/>
+        <v>-5.2500000000000003E-3</v>
+      </c>
+      <c r="C23" s="8">
+        <v>-1.0500000000000001E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.575E-2</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="7">
+        <v>44</v>
+      </c>
+      <c r="B24" s="8">
         <f t="shared" si="0"/>
-        <v>-0.155</v>
-      </c>
-      <c r="C24" s="7">
-        <v>-0.31</v>
-      </c>
-      <c r="D24" s="7">
+        <v>-5.1150000000000001E-2</v>
+      </c>
+      <c r="C24" s="8">
+        <v>-0.1023</v>
+      </c>
+      <c r="D24" s="8">
         <f t="shared" si="1"/>
-        <v>-0.46499999999999997</v>
+        <v>-0.15345</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="7">
+        <v>45</v>
+      </c>
+      <c r="B25" s="8">
         <f t="shared" si="0"/>
-        <v>-0.155</v>
-      </c>
-      <c r="C25" s="7">
-        <v>-0.31</v>
-      </c>
-      <c r="D25" s="7">
+        <v>-5.1150000000000001E-2</v>
+      </c>
+      <c r="C25" s="8">
+        <v>-0.1023</v>
+      </c>
+      <c r="D25" s="8">
         <f t="shared" si="1"/>
-        <v>-0.46499999999999997</v>
+        <v>-0.15345</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="7">
+        <v>46</v>
+      </c>
+      <c r="B26" s="8">
         <f t="shared" si="0"/>
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="C26" s="7">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="D26" s="7">
+        <v>-2.8500000000000001E-3</v>
+      </c>
+      <c r="C26" s="8">
+        <v>-5.7000000000000002E-3</v>
+      </c>
+      <c r="D26" s="8">
         <f t="shared" si="1"/>
-        <v>-0.42000000000000004</v>
+        <v>-8.5500000000000003E-3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B27" s="8">
         <f t="shared" si="0"/>
-        <v>-5.3E-3</v>
+        <v>-2.5999999999999998E-4</v>
       </c>
       <c r="C27" s="8">
-        <v>-1.06E-2</v>
+        <v>-5.1999999999999995E-4</v>
       </c>
       <c r="D27" s="8">
         <f t="shared" si="1"/>
-        <v>-1.5900000000000001E-2</v>
+        <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28" s="8">
         <f t="shared" si="0"/>
-        <v>-5.3E-3</v>
+        <v>-2.5999999999999998E-4</v>
       </c>
       <c r="C28" s="8">
-        <v>-1.06E-2</v>
+        <v>-5.1999999999999995E-4</v>
       </c>
       <c r="D28" s="8">
         <f t="shared" si="1"/>
-        <v>-1.5900000000000001E-2</v>
+        <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B29" s="8">
         <f t="shared" si="0"/>
-        <v>-5.1150000000000001E-2</v>
+        <v>-3.0499999999999999E-4</v>
       </c>
       <c r="C29" s="8">
-        <v>-0.1023</v>
+        <v>-6.0999999999999997E-4</v>
       </c>
       <c r="D29" s="8">
         <f t="shared" si="1"/>
-        <v>-0.15345</v>
+        <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="8">
         <f t="shared" si="0"/>
-        <v>-5.1150000000000001E-2</v>
+        <v>-3.0499999999999999E-4</v>
       </c>
       <c r="C30" s="8">
-        <v>-0.1023</v>
+        <v>-6.0999999999999997E-4</v>
       </c>
       <c r="D30" s="8">
         <f t="shared" si="1"/>
-        <v>-0.15345</v>
+        <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B31" s="8">
         <f t="shared" si="0"/>
-        <v>-2.8500000000000001E-3</v>
+        <v>-3.6999999999999999E-4</v>
       </c>
       <c r="C31" s="8">
-        <v>-5.7000000000000002E-3</v>
+        <v>-7.3999999999999999E-4</v>
       </c>
       <c r="D31" s="8">
         <f t="shared" si="1"/>
-        <v>-8.5500000000000003E-3</v>
+        <v>-1.1099999999999999E-3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="8">
-        <f t="shared" si="0"/>
-        <v>-2.5999999999999998E-4</v>
-      </c>
-      <c r="C32" s="8">
-        <v>-5.1999999999999995E-4</v>
-      </c>
-      <c r="D32" s="8">
-        <f t="shared" si="1"/>
-        <v>-7.7999999999999988E-4</v>
+        <v>26</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="8">
-        <f t="shared" si="0"/>
-        <v>-2.5999999999999998E-4</v>
-      </c>
-      <c r="C33" s="8">
-        <v>-5.1999999999999995E-4</v>
-      </c>
-      <c r="D33" s="8">
-        <f t="shared" si="1"/>
-        <v>-7.7999999999999988E-4</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>102</v>
+        <v>27</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="C33" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D33" s="9">
+        <v>-0.46</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="8">
-        <f t="shared" si="0"/>
-        <v>-3.0499999999999999E-4</v>
-      </c>
-      <c r="C34" s="8">
-        <v>-6.0999999999999997E-4</v>
-      </c>
-      <c r="D34" s="8">
-        <f t="shared" si="1"/>
-        <v>-9.1500000000000001E-4</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="8">
-        <f t="shared" si="0"/>
-        <v>-3.0499999999999999E-4</v>
-      </c>
-      <c r="C35" s="8">
-        <v>-6.0999999999999997E-4</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" si="1"/>
-        <v>-9.1500000000000001E-4</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="H35" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="8">
-        <f t="shared" si="0"/>
-        <v>-3.6999999999999999E-4</v>
-      </c>
-      <c r="C36" s="8">
-        <v>-7.3999999999999999E-4</v>
-      </c>
-      <c r="D36" s="8">
-        <f t="shared" si="1"/>
-        <v>-1.1099999999999999E-3</v>
+        <v>29</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.5</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="6">
-        <v>0</v>
-      </c>
-      <c r="C37" s="6">
-        <v>0</v>
-      </c>
-      <c r="D37" s="6">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="B37" s="10">
+        <v>250</v>
+      </c>
+      <c r="C37" s="10">
+        <v>1000</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2500</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>129</v>
+        <v>96</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="9">
-        <v>0.39</v>
-      </c>
-      <c r="C38" s="9">
-        <v>-0.02</v>
-      </c>
-      <c r="D38" s="9">
-        <v>-0.46</v>
+        <v>74</v>
+      </c>
+      <c r="B38" s="11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0.127</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0.23599999999999999</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="9">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D39" s="9">
-        <v>0.57999999999999996</v>
+        <v>75</v>
+      </c>
+      <c r="B39" s="11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C39" s="11">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0.14299999999999999</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1E-3</v>
-      </c>
-      <c r="C40" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="D40" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>74</v>
+      <c r="B40" s="11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C40" s="11">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="C41" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="E41" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C41" s="11">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>74</v>
+      <c r="F41" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B42" s="10">
-        <v>250</v>
-      </c>
-      <c r="C42" s="10">
-        <v>1000</v>
-      </c>
-      <c r="D42" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>74</v>
+        <v>78</v>
+      </c>
+      <c r="B42" s="11">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C42" s="11">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B43" s="11">
-        <v>2.1999999999999999E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C43" s="11">
-        <v>0.127</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="D43" s="11">
-        <v>0.23599999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B44" s="11">
         <v>5.5E-2</v>
@@ -2312,18 +2281,18 @@
         <v>31</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B45" s="11">
         <v>5.5E-2</v>
@@ -2338,18 +2307,18 @@
         <v>31</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B46" s="11">
         <v>5.5E-2</v>
@@ -2364,122 +2333,122 @@
         <v>31</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B47" s="11">
-        <v>5.5E-2</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C47" s="11">
-        <v>9.8999999999999977E-2</v>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D47" s="11">
-        <v>0.14299999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" s="11">
-        <v>8.2000000000000003E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C48" s="11">
-        <v>0.27200000000000002</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D48" s="11">
-        <v>0.49399999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B49" s="11">
-        <v>5.5E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C49" s="11">
-        <v>9.8999999999999977E-2</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="D49" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B50" s="11">
-        <v>5.5E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C50" s="11">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D50" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B51" s="11">
         <v>5.5E-2</v>
@@ -2494,122 +2463,125 @@
         <v>31</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" s="11">
-        <v>-1.0999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C52" s="11">
-        <v>2.8000000000000025E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D52" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B53" s="11">
-        <v>5.5E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C53" s="11">
-        <v>9.8999999999999977E-2</v>
+        <v>0.15900000000000003</v>
       </c>
       <c r="D53" s="11">
-        <v>0.14299999999999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B54" s="11">
-        <v>1.6E-2</v>
+        <f>B47</f>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C54" s="11">
-        <v>8.0000000000000071E-2</v>
+        <f t="shared" ref="C54:D54" si="2">C47</f>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D54" s="11">
-        <v>0.14799999999999999</v>
+        <f t="shared" si="2"/>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B55" s="11">
-        <v>4.9000000000000002E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C55" s="11">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D55" s="11">
-        <v>0.13200000000000001</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B56" s="11">
         <v>5.5E-2</v>
@@ -2624,18 +2596,18 @@
         <v>31</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B57" s="11">
         <v>5.5E-2</v>
@@ -2650,250 +2622,117 @@
         <v>31</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C58" s="11">
-        <v>0.15900000000000003</v>
-      </c>
-      <c r="D58" s="11">
-        <v>0.36299999999999999</v>
-      </c>
-      <c r="E58" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="C58" s="13">
+        <v>1</v>
+      </c>
+      <c r="D58" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F58" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="11">
-        <f>B52</f>
-        <v>-1.0999999999999999E-2</v>
-      </c>
-      <c r="C59" s="11">
-        <f t="shared" ref="C59:D59" si="2">C52</f>
-        <v>2.8000000000000025E-2</v>
-      </c>
-      <c r="D59" s="11">
-        <f t="shared" si="2"/>
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="E59" s="5" t="s">
+      <c r="F58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="1">
+        <v>12.84</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>136.03</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="1">
+        <v>50</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1">
+        <v>150</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="13">
+        <v>0.33</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.66</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F59" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="11">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C60" s="11">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D60" s="11">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="11">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C61" s="11">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D61" s="11">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="11">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C62" s="11">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D62" s="11">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B63" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="C63" s="13">
-        <v>1</v>
-      </c>
-      <c r="D63" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="1">
-        <v>12.84</v>
-      </c>
-      <c r="C64" s="1">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1">
-        <v>136.03</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B65" s="1">
-        <v>50</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1">
-        <v>150</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B66" s="13">
-        <v>0.33</v>
-      </c>
-      <c r="C66" s="1">
-        <v>0</v>
-      </c>
-      <c r="D66" s="13">
-        <v>0.66</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>64</v>
+      <c r="F61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2918,7 +2757,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,221 +2765,221 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sensitivity analysis parameter updates
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE87B44B-A1B1-4F3F-842E-8C47A62736F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F6C98-D336-4BFE-ADEB-75140FF7646E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter values" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -513,9 +513,6 @@
     <t>$/t biochar</t>
   </si>
   <si>
-    <t>config files made</t>
-  </si>
-  <si>
     <t>CarbonTaxLow</t>
   </si>
   <si>
@@ -564,22 +561,7 @@
     <t>in db</t>
   </si>
   <si>
-    <t>will likely error</t>
-  </si>
-  <si>
-    <t>running</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
     <t>error</t>
-  </si>
-  <si>
-    <t>in R</t>
-  </si>
-  <si>
-    <t>need to replace 2062</t>
   </si>
 </sst>
 </file>
@@ -627,7 +609,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -642,12 +624,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -655,12 +631,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,7 +700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -768,11 +738,9 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1169,13 +1137,13 @@
         <v>65</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1251,13 +1219,13 @@
         <v>65</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1341,7 +1309,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1423,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1501,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,13 +1533,13 @@
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>34</v>
@@ -1591,13 +1559,13 @@
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>34</v>
@@ -2764,7 +2732,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,228 +2759,217 @@
       <c r="A3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>159</v>
+      <c r="B3" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>159</v>
+      <c r="B4" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>159</v>
+      <c r="B5" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>159</v>
+      <c r="B6" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>163</v>
+      <c r="B7" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>159</v>
+      <c r="B8" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>159</v>
+      <c r="B9" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>159</v>
+      <c r="B10" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="D11" s="14"/>
+      <c r="B11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>159</v>
+      <c r="B12" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>161</v>
+      <c r="B13" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>159</v>
+      <c r="B14" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C15" s="14"/>
+      <c r="B15" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>159</v>
+      <c r="B17" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>159</v>
+      <c r="B19" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>159</v>
+      <c r="B20" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>159</v>
+      <c r="B21" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>159</v>
+      <c r="B22" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" t="s">
         <v>143</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>165</v>
-      </c>
+      <c r="B23" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>145</v>
-      </c>
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>160</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>146</v>
-      </c>
-      <c r="B25" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>160</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>160</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B27" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="13"/>
+        <v>147</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B28" t="s">
-        <v>162</v>
+        <v>148</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>